<commit_message>
Actualizar la forma en la que se encuentran presentados los datos
</commit_message>
<xml_diff>
--- a/app/Datos/Intermodal/Costos e Inversiones.xlsx
+++ b/app/Datos/Intermodal/Costos e Inversiones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Egresos" sheetId="1" r:id="rId1"/>
@@ -454,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4907,8 +4907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DJ22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11455,7 +11455,7 @@
     </row>
     <row r="20" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
@@ -12143,7 +12143,7 @@
     </row>
     <row r="22" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Cambie el nombre de la hoja de egresos por costos
</commit_message>
<xml_diff>
--- a/app/Datos/Intermodal/Costos e Inversiones.xlsx
+++ b/app/Datos/Intermodal/Costos e Inversiones.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Egresos" sheetId="1" r:id="rId1"/>
+    <sheet name="Costos" sheetId="1" r:id="rId1"/>
     <sheet name="Inversiones" sheetId="2" r:id="rId2"/>
     <sheet name="Notas" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -454,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DI13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -4907,8 +4907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Correcion valores de Costos e Inversiones
</commit_message>
<xml_diff>
--- a/app/Datos/Intermodal/Costos e Inversiones.xlsx
+++ b/app/Datos/Intermodal/Costos e Inversiones.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:DI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A19" sqref="A19:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,313 +1514,313 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>15331</v>
+        <v>7665.5</v>
       </c>
       <c r="L4">
-        <v>15714</v>
+        <v>7857</v>
       </c>
       <c r="M4">
-        <v>16107</v>
+        <v>8053.5</v>
       </c>
       <c r="N4">
-        <v>16510</v>
+        <v>8255</v>
       </c>
       <c r="O4">
-        <v>16923</v>
+        <v>8461.5</v>
       </c>
       <c r="P4">
-        <v>17346</v>
+        <v>8673</v>
       </c>
       <c r="Q4">
-        <v>17779</v>
+        <v>8889.5</v>
       </c>
       <c r="R4">
-        <v>18224</v>
+        <v>9112</v>
       </c>
       <c r="S4">
-        <v>18679</v>
+        <v>9339.5</v>
       </c>
       <c r="T4">
-        <v>19146</v>
+        <v>9573</v>
       </c>
       <c r="U4">
-        <v>19625</v>
+        <v>9812.5</v>
       </c>
       <c r="V4">
-        <v>26819</v>
+        <v>13409.5</v>
       </c>
       <c r="W4">
-        <v>27489</v>
+        <v>13744.5</v>
       </c>
       <c r="X4">
-        <v>28176</v>
+        <v>14088</v>
       </c>
       <c r="Y4">
-        <v>28881</v>
+        <v>14440.5</v>
       </c>
       <c r="Z4">
-        <v>29603</v>
+        <v>14801.5</v>
       </c>
       <c r="AA4">
-        <v>30343</v>
+        <v>15171.5</v>
       </c>
       <c r="AB4">
-        <v>31101</v>
+        <v>15550.5</v>
       </c>
       <c r="AC4">
-        <v>31879</v>
+        <v>15939.5</v>
       </c>
       <c r="AD4">
-        <v>32676</v>
+        <v>16338</v>
       </c>
       <c r="AE4">
-        <v>33493</v>
+        <v>16746.5</v>
       </c>
       <c r="AF4">
-        <v>34330</v>
+        <v>17165</v>
       </c>
       <c r="AG4">
-        <v>35188</v>
+        <v>17594</v>
       </c>
       <c r="AH4">
-        <v>36068</v>
+        <v>18034</v>
       </c>
       <c r="AI4">
-        <v>36970</v>
+        <v>18485</v>
       </c>
       <c r="AJ4">
-        <v>43820</v>
+        <v>21910</v>
       </c>
       <c r="AK4">
-        <v>44916</v>
+        <v>22458</v>
       </c>
       <c r="AL4">
-        <v>46039</v>
+        <v>23019.5</v>
       </c>
       <c r="AM4">
-        <v>47190</v>
+        <v>23595</v>
       </c>
       <c r="AN4">
-        <v>48369</v>
+        <v>24184.5</v>
       </c>
       <c r="AO4">
-        <v>49579</v>
+        <v>24789.5</v>
       </c>
       <c r="AP4">
-        <v>50818</v>
+        <v>25409</v>
       </c>
       <c r="AQ4">
-        <v>52089</v>
+        <v>26044.5</v>
       </c>
       <c r="AR4">
-        <v>53391</v>
+        <v>26695.5</v>
       </c>
       <c r="AS4">
-        <v>54726</v>
+        <v>27363</v>
       </c>
       <c r="AT4">
-        <v>56094</v>
+        <v>28047</v>
       </c>
       <c r="AU4">
-        <v>57496</v>
+        <v>28748</v>
       </c>
       <c r="AV4">
-        <v>58933</v>
+        <v>29466.5</v>
       </c>
       <c r="AW4">
-        <v>60407</v>
+        <v>30203.5</v>
       </c>
       <c r="AX4">
-        <v>61917</v>
+        <v>30958.5</v>
       </c>
       <c r="AY4">
-        <v>63465</v>
+        <v>31732.5</v>
       </c>
       <c r="AZ4">
-        <v>65051</v>
+        <v>32525.5</v>
       </c>
       <c r="BA4">
-        <v>66678</v>
+        <v>33339</v>
       </c>
       <c r="BB4">
-        <v>68345</v>
+        <v>34172.5</v>
       </c>
       <c r="BC4">
-        <v>70053</v>
+        <v>35026.5</v>
       </c>
       <c r="BD4">
-        <v>71805</v>
+        <v>35902.5</v>
       </c>
       <c r="BE4">
-        <v>73600</v>
+        <v>36800</v>
       </c>
       <c r="BF4">
-        <v>75440</v>
+        <v>37720</v>
       </c>
       <c r="BG4">
-        <v>77326</v>
+        <v>38663</v>
       </c>
       <c r="BH4">
-        <v>79259</v>
+        <v>39629.5</v>
       </c>
       <c r="BI4">
-        <v>81240</v>
+        <v>40620</v>
       </c>
       <c r="BJ4">
-        <v>83271</v>
+        <v>41635.5</v>
       </c>
       <c r="BK4">
-        <v>85353</v>
+        <v>42676.5</v>
       </c>
       <c r="BL4">
-        <v>87487</v>
+        <v>43743.5</v>
       </c>
       <c r="BM4">
-        <v>89674</v>
+        <v>44837</v>
       </c>
       <c r="BN4">
-        <v>91916</v>
+        <v>45958</v>
       </c>
       <c r="BO4">
-        <v>94214</v>
+        <v>47107</v>
       </c>
       <c r="BP4">
-        <v>96569</v>
+        <v>48284.5</v>
       </c>
       <c r="BQ4">
-        <v>98984</v>
+        <v>49492</v>
       </c>
       <c r="BR4">
-        <v>101458</v>
+        <v>50729</v>
       </c>
       <c r="BS4">
-        <v>103995</v>
+        <v>51997.5</v>
       </c>
       <c r="BT4">
-        <v>106594</v>
+        <v>53297</v>
       </c>
       <c r="BU4">
-        <v>109259</v>
+        <v>54629.5</v>
       </c>
       <c r="BV4">
-        <v>111991</v>
+        <v>55995.5</v>
       </c>
       <c r="BW4">
-        <v>114791</v>
+        <v>57395.5</v>
       </c>
       <c r="BX4">
-        <v>117660</v>
+        <v>58830</v>
       </c>
       <c r="BY4">
-        <v>120602</v>
+        <v>60301</v>
       </c>
       <c r="BZ4">
-        <v>123617</v>
+        <v>61808.5</v>
       </c>
       <c r="CA4">
-        <v>126707</v>
+        <v>63353.5</v>
       </c>
       <c r="CB4">
-        <v>129875</v>
+        <v>64937.5</v>
       </c>
       <c r="CC4">
-        <v>133122</v>
+        <v>66561</v>
       </c>
       <c r="CD4">
-        <v>136450</v>
+        <v>68225</v>
       </c>
       <c r="CE4">
-        <v>139861</v>
+        <v>69930.5</v>
       </c>
       <c r="CF4">
-        <v>143358</v>
+        <v>71679</v>
       </c>
       <c r="CG4">
-        <v>146942</v>
+        <v>73471</v>
       </c>
       <c r="CH4">
-        <v>150615</v>
+        <v>75307.5</v>
       </c>
       <c r="CI4">
-        <v>154381</v>
+        <v>77190.5</v>
       </c>
       <c r="CJ4">
-        <v>158240</v>
+        <v>79120</v>
       </c>
       <c r="CK4">
-        <v>162196</v>
+        <v>81098</v>
       </c>
       <c r="CL4">
-        <v>166251</v>
+        <v>83125.5</v>
       </c>
       <c r="CM4">
-        <v>170407</v>
+        <v>85203.5</v>
       </c>
       <c r="CN4">
-        <v>174667</v>
+        <v>87333.5</v>
       </c>
       <c r="CO4">
-        <v>179034</v>
+        <v>89517</v>
       </c>
       <c r="CP4">
-        <v>183510</v>
+        <v>91755</v>
       </c>
       <c r="CQ4">
-        <v>188098</v>
+        <v>94049</v>
       </c>
       <c r="CR4">
-        <v>192800</v>
+        <v>96400</v>
       </c>
       <c r="CS4">
-        <v>197620</v>
+        <v>98810</v>
       </c>
       <c r="CT4">
-        <v>202561</v>
+        <v>101280.5</v>
       </c>
       <c r="CU4">
-        <v>207625</v>
+        <v>103812.5</v>
       </c>
       <c r="CV4">
-        <v>212815</v>
+        <v>106407.5</v>
       </c>
       <c r="CW4">
-        <v>218136</v>
+        <v>109068</v>
       </c>
       <c r="CX4">
-        <v>223589</v>
+        <v>111794.5</v>
       </c>
       <c r="CY4">
-        <v>229179</v>
+        <v>114589.5</v>
       </c>
       <c r="CZ4">
-        <v>234908</v>
+        <v>117454</v>
       </c>
       <c r="DA4">
-        <v>240781</v>
+        <v>120390.5</v>
       </c>
       <c r="DB4">
-        <v>246800</v>
+        <v>123400</v>
       </c>
       <c r="DC4">
-        <v>252970</v>
+        <v>126485</v>
       </c>
       <c r="DD4">
-        <v>259295</v>
+        <v>129647.5</v>
       </c>
       <c r="DE4">
-        <v>265777</v>
+        <v>132888.5</v>
       </c>
       <c r="DF4">
-        <v>272422</v>
+        <v>136211</v>
       </c>
       <c r="DG4">
-        <v>279232</v>
+        <v>139616</v>
       </c>
       <c r="DH4">
-        <v>286213</v>
+        <v>143106.5</v>
       </c>
       <c r="DI4">
-        <v>293368</v>
+        <v>146684</v>
       </c>
     </row>
     <row r="5" spans="1:113" x14ac:dyDescent="0.2">
@@ -1837,439 +1837,330 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <f>E4*0.5</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:BQ5" si="0">F4*0.5</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
         <v>7665.5</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
         <v>7857</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
         <v>8053.5</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
         <v>8255</v>
       </c>
       <c r="O5">
-        <f t="shared" si="0"/>
         <v>8461.5</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
         <v>8673</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
         <v>8889.5</v>
       </c>
       <c r="R5">
-        <f t="shared" si="0"/>
         <v>9112</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
         <v>9339.5</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
         <v>9573</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
         <v>9812.5</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
         <v>13409.5</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
         <v>13744.5</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
         <v>14088</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="0"/>
         <v>14440.5</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="0"/>
         <v>14801.5</v>
       </c>
       <c r="AA5">
-        <f t="shared" si="0"/>
         <v>15171.5</v>
       </c>
       <c r="AB5">
-        <f t="shared" si="0"/>
         <v>15550.5</v>
       </c>
       <c r="AC5">
-        <f t="shared" si="0"/>
         <v>15939.5</v>
       </c>
       <c r="AD5">
-        <f t="shared" si="0"/>
         <v>16338</v>
       </c>
       <c r="AE5">
-        <f t="shared" si="0"/>
         <v>16746.5</v>
       </c>
       <c r="AF5">
-        <f t="shared" si="0"/>
         <v>17165</v>
       </c>
       <c r="AG5">
-        <f t="shared" si="0"/>
         <v>17594</v>
       </c>
       <c r="AH5">
-        <f t="shared" si="0"/>
         <v>18034</v>
       </c>
       <c r="AI5">
-        <f t="shared" si="0"/>
         <v>18485</v>
       </c>
       <c r="AJ5">
-        <f t="shared" si="0"/>
         <v>21910</v>
       </c>
       <c r="AK5">
-        <f t="shared" si="0"/>
         <v>22458</v>
       </c>
       <c r="AL5">
-        <f t="shared" si="0"/>
         <v>23019.5</v>
       </c>
       <c r="AM5">
-        <f t="shared" si="0"/>
         <v>23595</v>
       </c>
       <c r="AN5">
-        <f t="shared" si="0"/>
         <v>24184.5</v>
       </c>
       <c r="AO5">
-        <f t="shared" si="0"/>
         <v>24789.5</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
         <v>25409</v>
       </c>
       <c r="AQ5">
-        <f t="shared" si="0"/>
         <v>26044.5</v>
       </c>
       <c r="AR5">
-        <f t="shared" si="0"/>
         <v>26695.5</v>
       </c>
       <c r="AS5">
-        <f t="shared" si="0"/>
         <v>27363</v>
       </c>
       <c r="AT5">
-        <f t="shared" si="0"/>
         <v>28047</v>
       </c>
       <c r="AU5">
-        <f t="shared" si="0"/>
         <v>28748</v>
       </c>
       <c r="AV5">
-        <f t="shared" si="0"/>
         <v>29466.5</v>
       </c>
       <c r="AW5">
-        <f t="shared" si="0"/>
         <v>30203.5</v>
       </c>
       <c r="AX5">
-        <f t="shared" si="0"/>
         <v>30958.5</v>
       </c>
       <c r="AY5">
-        <f t="shared" si="0"/>
         <v>31732.5</v>
       </c>
       <c r="AZ5">
-        <f t="shared" si="0"/>
         <v>32525.5</v>
       </c>
       <c r="BA5">
-        <f t="shared" si="0"/>
         <v>33339</v>
       </c>
       <c r="BB5">
-        <f t="shared" si="0"/>
         <v>34172.5</v>
       </c>
       <c r="BC5">
-        <f t="shared" si="0"/>
         <v>35026.5</v>
       </c>
       <c r="BD5">
-        <f t="shared" si="0"/>
         <v>35902.5</v>
       </c>
       <c r="BE5">
-        <f t="shared" si="0"/>
         <v>36800</v>
       </c>
       <c r="BF5">
-        <f t="shared" si="0"/>
         <v>37720</v>
       </c>
       <c r="BG5">
-        <f t="shared" si="0"/>
         <v>38663</v>
       </c>
       <c r="BH5">
-        <f t="shared" si="0"/>
         <v>39629.5</v>
       </c>
       <c r="BI5">
-        <f t="shared" si="0"/>
         <v>40620</v>
       </c>
       <c r="BJ5">
-        <f t="shared" si="0"/>
         <v>41635.5</v>
       </c>
       <c r="BK5">
-        <f t="shared" si="0"/>
         <v>42676.5</v>
       </c>
       <c r="BL5">
-        <f t="shared" si="0"/>
         <v>43743.5</v>
       </c>
       <c r="BM5">
-        <f t="shared" si="0"/>
         <v>44837</v>
       </c>
       <c r="BN5">
-        <f t="shared" si="0"/>
         <v>45958</v>
       </c>
       <c r="BO5">
-        <f t="shared" si="0"/>
         <v>47107</v>
       </c>
       <c r="BP5">
-        <f t="shared" si="0"/>
         <v>48284.5</v>
       </c>
       <c r="BQ5">
-        <f t="shared" si="0"/>
         <v>49492</v>
       </c>
       <c r="BR5">
-        <f t="shared" ref="BR5:DI5" si="1">BR4*0.5</f>
         <v>50729</v>
       </c>
       <c r="BS5">
-        <f t="shared" si="1"/>
         <v>51997.5</v>
       </c>
       <c r="BT5">
-        <f t="shared" si="1"/>
         <v>53297</v>
       </c>
       <c r="BU5">
-        <f t="shared" si="1"/>
         <v>54629.5</v>
       </c>
       <c r="BV5">
-        <f t="shared" si="1"/>
         <v>55995.5</v>
       </c>
       <c r="BW5">
-        <f t="shared" si="1"/>
         <v>57395.5</v>
       </c>
       <c r="BX5">
-        <f t="shared" si="1"/>
         <v>58830</v>
       </c>
       <c r="BY5">
-        <f t="shared" si="1"/>
         <v>60301</v>
       </c>
       <c r="BZ5">
-        <f t="shared" si="1"/>
         <v>61808.5</v>
       </c>
       <c r="CA5">
-        <f t="shared" si="1"/>
         <v>63353.5</v>
       </c>
       <c r="CB5">
-        <f t="shared" si="1"/>
         <v>64937.5</v>
       </c>
       <c r="CC5">
-        <f t="shared" si="1"/>
         <v>66561</v>
       </c>
       <c r="CD5">
-        <f t="shared" si="1"/>
         <v>68225</v>
       </c>
       <c r="CE5">
-        <f t="shared" si="1"/>
         <v>69930.5</v>
       </c>
       <c r="CF5">
-        <f t="shared" si="1"/>
         <v>71679</v>
       </c>
       <c r="CG5">
-        <f t="shared" si="1"/>
         <v>73471</v>
       </c>
       <c r="CH5">
-        <f t="shared" si="1"/>
         <v>75307.5</v>
       </c>
       <c r="CI5">
-        <f t="shared" si="1"/>
         <v>77190.5</v>
       </c>
       <c r="CJ5">
-        <f t="shared" si="1"/>
         <v>79120</v>
       </c>
       <c r="CK5">
-        <f t="shared" si="1"/>
         <v>81098</v>
       </c>
       <c r="CL5">
-        <f t="shared" si="1"/>
         <v>83125.5</v>
       </c>
       <c r="CM5">
-        <f t="shared" si="1"/>
         <v>85203.5</v>
       </c>
       <c r="CN5">
-        <f t="shared" si="1"/>
         <v>87333.5</v>
       </c>
       <c r="CO5">
-        <f t="shared" si="1"/>
         <v>89517</v>
       </c>
       <c r="CP5">
-        <f t="shared" si="1"/>
         <v>91755</v>
       </c>
       <c r="CQ5">
-        <f t="shared" si="1"/>
         <v>94049</v>
       </c>
       <c r="CR5">
-        <f t="shared" si="1"/>
         <v>96400</v>
       </c>
       <c r="CS5">
-        <f t="shared" si="1"/>
         <v>98810</v>
       </c>
       <c r="CT5">
-        <f t="shared" si="1"/>
         <v>101280.5</v>
       </c>
       <c r="CU5">
-        <f t="shared" si="1"/>
         <v>103812.5</v>
       </c>
       <c r="CV5">
-        <f t="shared" si="1"/>
         <v>106407.5</v>
       </c>
       <c r="CW5">
-        <f t="shared" si="1"/>
         <v>109068</v>
       </c>
       <c r="CX5">
-        <f t="shared" si="1"/>
         <v>111794.5</v>
       </c>
       <c r="CY5">
-        <f t="shared" si="1"/>
         <v>114589.5</v>
       </c>
       <c r="CZ5">
-        <f t="shared" si="1"/>
         <v>117454</v>
       </c>
       <c r="DA5">
-        <f t="shared" si="1"/>
         <v>120390.5</v>
       </c>
       <c r="DB5">
-        <f t="shared" si="1"/>
         <v>123400</v>
       </c>
       <c r="DC5">
-        <f t="shared" si="1"/>
         <v>126485</v>
       </c>
       <c r="DD5">
-        <f t="shared" si="1"/>
         <v>129647.5</v>
       </c>
       <c r="DE5">
-        <f t="shared" si="1"/>
         <v>132888.5</v>
       </c>
       <c r="DF5">
-        <f t="shared" si="1"/>
         <v>136211</v>
       </c>
       <c r="DG5">
-        <f t="shared" si="1"/>
         <v>139616</v>
       </c>
       <c r="DH5">
-        <f t="shared" si="1"/>
         <v>143106.5</v>
       </c>
       <c r="DI5">
-        <f t="shared" si="1"/>
         <v>146684</v>
       </c>
     </row>
@@ -2305,313 +2196,313 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>25514</v>
+        <v>12757</v>
       </c>
       <c r="L6">
-        <v>26152</v>
+        <v>13076</v>
       </c>
       <c r="M6">
-        <v>26806</v>
+        <v>13403</v>
       </c>
       <c r="N6">
-        <v>27476</v>
+        <v>13738</v>
       </c>
       <c r="O6">
-        <v>28163</v>
+        <v>14081.5</v>
       </c>
       <c r="P6">
-        <v>28867</v>
+        <v>14433.5</v>
       </c>
       <c r="Q6">
-        <v>29589</v>
+        <v>14794.5</v>
       </c>
       <c r="R6">
-        <v>30328</v>
+        <v>15164</v>
       </c>
       <c r="S6">
-        <v>31087</v>
+        <v>15543.5</v>
       </c>
       <c r="T6">
-        <v>31864</v>
+        <v>15932</v>
       </c>
       <c r="U6">
-        <v>32660</v>
+        <v>16330</v>
       </c>
       <c r="V6">
-        <v>43144</v>
+        <v>21572</v>
       </c>
       <c r="W6">
-        <v>44223</v>
+        <v>22111.5</v>
       </c>
       <c r="X6">
-        <v>45328</v>
+        <v>22664</v>
       </c>
       <c r="Y6">
-        <v>46461</v>
+        <v>23230.5</v>
       </c>
       <c r="Z6">
-        <v>47623</v>
+        <v>23811.5</v>
       </c>
       <c r="AA6">
-        <v>48814</v>
+        <v>24407</v>
       </c>
       <c r="AB6">
-        <v>50034</v>
+        <v>25017</v>
       </c>
       <c r="AC6">
-        <v>51285</v>
+        <v>25642.5</v>
       </c>
       <c r="AD6">
-        <v>52567</v>
+        <v>26283.5</v>
       </c>
       <c r="AE6">
-        <v>53881</v>
+        <v>26940.5</v>
       </c>
       <c r="AF6">
-        <v>55228</v>
+        <v>27614</v>
       </c>
       <c r="AG6">
-        <v>56609</v>
+        <v>28304.5</v>
       </c>
       <c r="AH6">
-        <v>58024</v>
+        <v>29012</v>
       </c>
       <c r="AI6">
-        <v>59475</v>
+        <v>29737.5</v>
       </c>
       <c r="AJ6">
-        <v>75137</v>
+        <v>37568.5</v>
       </c>
       <c r="AK6">
-        <v>77015</v>
+        <v>38507.5</v>
       </c>
       <c r="AL6">
-        <v>78941</v>
+        <v>39470.5</v>
       </c>
       <c r="AM6">
-        <v>80914</v>
+        <v>40457</v>
       </c>
       <c r="AN6">
-        <v>82937</v>
+        <v>41468.5</v>
       </c>
       <c r="AO6">
-        <v>85010</v>
+        <v>42505</v>
       </c>
       <c r="AP6">
-        <v>87136</v>
+        <v>43568</v>
       </c>
       <c r="AQ6">
-        <v>89314</v>
+        <v>44657</v>
       </c>
       <c r="AR6">
-        <v>91547</v>
+        <v>45773.5</v>
       </c>
       <c r="AS6">
-        <v>93835</v>
+        <v>46917.5</v>
       </c>
       <c r="AT6">
-        <v>96181</v>
+        <v>48090.5</v>
       </c>
       <c r="AU6">
-        <v>98586</v>
+        <v>49293</v>
       </c>
       <c r="AV6">
-        <v>101051</v>
+        <v>50525.5</v>
       </c>
       <c r="AW6">
-        <v>103577</v>
+        <v>51788.5</v>
       </c>
       <c r="AX6">
-        <v>106166</v>
+        <v>53083</v>
       </c>
       <c r="AY6">
-        <v>108820</v>
+        <v>54410</v>
       </c>
       <c r="AZ6">
-        <v>111541</v>
+        <v>55770.5</v>
       </c>
       <c r="BA6">
-        <v>114329</v>
+        <v>57164.5</v>
       </c>
       <c r="BB6">
-        <v>117188</v>
+        <v>58594</v>
       </c>
       <c r="BC6">
-        <v>120117</v>
+        <v>60058.5</v>
       </c>
       <c r="BD6">
-        <v>123120</v>
+        <v>61560</v>
       </c>
       <c r="BE6">
-        <v>126198</v>
+        <v>63099</v>
       </c>
       <c r="BF6">
-        <v>129353</v>
+        <v>64676.5</v>
       </c>
       <c r="BG6">
-        <v>132587</v>
+        <v>66293.5</v>
       </c>
       <c r="BH6">
-        <v>135902</v>
+        <v>67951</v>
       </c>
       <c r="BI6">
-        <v>139299</v>
+        <v>69649.5</v>
       </c>
       <c r="BJ6">
-        <v>142782</v>
+        <v>71391</v>
       </c>
       <c r="BK6">
-        <v>146351</v>
+        <v>73175.5</v>
       </c>
       <c r="BL6">
-        <v>150010</v>
+        <v>75005</v>
       </c>
       <c r="BM6">
-        <v>153760</v>
+        <v>76880</v>
       </c>
       <c r="BN6">
-        <v>157604</v>
+        <v>78802</v>
       </c>
       <c r="BO6">
-        <v>161545</v>
+        <v>80772.5</v>
       </c>
       <c r="BP6">
-        <v>165583</v>
+        <v>82791.5</v>
       </c>
       <c r="BQ6">
-        <v>169723</v>
+        <v>84861.5</v>
       </c>
       <c r="BR6">
-        <v>173966</v>
+        <v>86983</v>
       </c>
       <c r="BS6">
-        <v>178315</v>
+        <v>89157.5</v>
       </c>
       <c r="BT6">
-        <v>182773</v>
+        <v>91386.5</v>
       </c>
       <c r="BU6">
-        <v>187342</v>
+        <v>93671</v>
       </c>
       <c r="BV6">
-        <v>192026</v>
+        <v>96013</v>
       </c>
       <c r="BW6">
-        <v>196826</v>
+        <v>98413</v>
       </c>
       <c r="BX6">
-        <v>201747</v>
+        <v>100873.5</v>
       </c>
       <c r="BY6">
-        <v>206791</v>
+        <v>103395.5</v>
       </c>
       <c r="BZ6">
-        <v>211960</v>
+        <v>105980</v>
       </c>
       <c r="CA6">
-        <v>217259</v>
+        <v>108629.5</v>
       </c>
       <c r="CB6">
-        <v>222691</v>
+        <v>111345.5</v>
       </c>
       <c r="CC6">
-        <v>228258</v>
+        <v>114129</v>
       </c>
       <c r="CD6">
-        <v>233965</v>
+        <v>116982.5</v>
       </c>
       <c r="CE6">
-        <v>239814</v>
+        <v>119907</v>
       </c>
       <c r="CF6">
-        <v>245809</v>
+        <v>122904.5</v>
       </c>
       <c r="CG6">
-        <v>251954</v>
+        <v>125977</v>
       </c>
       <c r="CH6">
-        <v>258253</v>
+        <v>129126.5</v>
       </c>
       <c r="CI6">
-        <v>264709</v>
+        <v>132354.5</v>
       </c>
       <c r="CJ6">
-        <v>271327</v>
+        <v>135663.5</v>
       </c>
       <c r="CK6">
-        <v>278110</v>
+        <v>139055</v>
       </c>
       <c r="CL6">
-        <v>285063</v>
+        <v>142531.5</v>
       </c>
       <c r="CM6">
-        <v>292190</v>
+        <v>146095</v>
       </c>
       <c r="CN6">
-        <v>299494</v>
+        <v>149747</v>
       </c>
       <c r="CO6">
-        <v>306982</v>
+        <v>153491</v>
       </c>
       <c r="CP6">
-        <v>314656</v>
+        <v>157328</v>
       </c>
       <c r="CQ6">
-        <v>322523</v>
+        <v>161261.5</v>
       </c>
       <c r="CR6">
-        <v>330586</v>
+        <v>165293</v>
       </c>
       <c r="CS6">
-        <v>338851</v>
+        <v>169425.5</v>
       </c>
       <c r="CT6">
-        <v>347322</v>
+        <v>173661</v>
       </c>
       <c r="CU6">
-        <v>356005</v>
+        <v>178002.5</v>
       </c>
       <c r="CV6">
-        <v>364905</v>
+        <v>182452.5</v>
       </c>
       <c r="CW6">
-        <v>374028</v>
+        <v>187014</v>
       </c>
       <c r="CX6">
-        <v>383378</v>
+        <v>191689</v>
       </c>
       <c r="CY6">
-        <v>392963</v>
+        <v>196481.5</v>
       </c>
       <c r="CZ6">
-        <v>402787</v>
+        <v>201393.5</v>
       </c>
       <c r="DA6">
-        <v>412856</v>
+        <v>206428</v>
       </c>
       <c r="DB6">
-        <v>423178</v>
+        <v>211589</v>
       </c>
       <c r="DC6">
-        <v>433757</v>
+        <v>216878.5</v>
       </c>
       <c r="DD6">
-        <v>444601</v>
+        <v>222300.5</v>
       </c>
       <c r="DE6">
-        <v>455716</v>
+        <v>227858</v>
       </c>
       <c r="DF6">
-        <v>467109</v>
+        <v>233554.5</v>
       </c>
       <c r="DG6">
-        <v>478787</v>
+        <v>239393.5</v>
       </c>
       <c r="DH6">
-        <v>490757</v>
+        <v>245378.5</v>
       </c>
       <c r="DI6">
-        <v>503025</v>
+        <v>251512.5</v>
       </c>
     </row>
     <row r="7" spans="1:113" x14ac:dyDescent="0.2">
@@ -2628,439 +2519,330 @@
         <v>11</v>
       </c>
       <c r="E7">
-        <f>E6*0.5</f>
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7:BQ7" si="2">F6*0.5</f>
         <v>0</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
         <v>12757</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
         <v>13076</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
         <v>13403</v>
       </c>
       <c r="N7">
-        <f t="shared" si="2"/>
         <v>13738</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
         <v>14081.5</v>
       </c>
       <c r="P7">
-        <f t="shared" si="2"/>
         <v>14433.5</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="2"/>
         <v>14794.5</v>
       </c>
       <c r="R7">
-        <f t="shared" si="2"/>
         <v>15164</v>
       </c>
       <c r="S7">
-        <f t="shared" si="2"/>
         <v>15543.5</v>
       </c>
       <c r="T7">
-        <f t="shared" si="2"/>
         <v>15932</v>
       </c>
       <c r="U7">
-        <f t="shared" si="2"/>
         <v>16330</v>
       </c>
       <c r="V7">
-        <f t="shared" si="2"/>
         <v>21572</v>
       </c>
       <c r="W7">
-        <f t="shared" si="2"/>
         <v>22111.5</v>
       </c>
       <c r="X7">
-        <f t="shared" si="2"/>
         <v>22664</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="2"/>
         <v>23230.5</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="2"/>
         <v>23811.5</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="2"/>
         <v>24407</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="2"/>
         <v>25017</v>
       </c>
       <c r="AC7">
-        <f t="shared" si="2"/>
         <v>25642.5</v>
       </c>
       <c r="AD7">
-        <f t="shared" si="2"/>
         <v>26283.5</v>
       </c>
       <c r="AE7">
-        <f t="shared" si="2"/>
         <v>26940.5</v>
       </c>
       <c r="AF7">
-        <f t="shared" si="2"/>
         <v>27614</v>
       </c>
       <c r="AG7">
-        <f t="shared" si="2"/>
         <v>28304.5</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="2"/>
         <v>29012</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="2"/>
         <v>29737.5</v>
       </c>
       <c r="AJ7">
-        <f t="shared" si="2"/>
         <v>37568.5</v>
       </c>
       <c r="AK7">
-        <f t="shared" si="2"/>
         <v>38507.5</v>
       </c>
       <c r="AL7">
-        <f t="shared" si="2"/>
         <v>39470.5</v>
       </c>
       <c r="AM7">
-        <f t="shared" si="2"/>
         <v>40457</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="2"/>
         <v>41468.5</v>
       </c>
       <c r="AO7">
-        <f t="shared" si="2"/>
         <v>42505</v>
       </c>
       <c r="AP7">
-        <f t="shared" si="2"/>
         <v>43568</v>
       </c>
       <c r="AQ7">
-        <f t="shared" si="2"/>
         <v>44657</v>
       </c>
       <c r="AR7">
-        <f t="shared" si="2"/>
         <v>45773.5</v>
       </c>
       <c r="AS7">
-        <f t="shared" si="2"/>
         <v>46917.5</v>
       </c>
       <c r="AT7">
-        <f t="shared" si="2"/>
         <v>48090.5</v>
       </c>
       <c r="AU7">
-        <f t="shared" si="2"/>
         <v>49293</v>
       </c>
       <c r="AV7">
-        <f t="shared" si="2"/>
         <v>50525.5</v>
       </c>
       <c r="AW7">
-        <f t="shared" si="2"/>
         <v>51788.5</v>
       </c>
       <c r="AX7">
-        <f t="shared" si="2"/>
         <v>53083</v>
       </c>
       <c r="AY7">
-        <f t="shared" si="2"/>
         <v>54410</v>
       </c>
       <c r="AZ7">
-        <f t="shared" si="2"/>
         <v>55770.5</v>
       </c>
       <c r="BA7">
-        <f t="shared" si="2"/>
         <v>57164.5</v>
       </c>
       <c r="BB7">
-        <f t="shared" si="2"/>
         <v>58594</v>
       </c>
       <c r="BC7">
-        <f t="shared" si="2"/>
         <v>60058.5</v>
       </c>
       <c r="BD7">
-        <f t="shared" si="2"/>
         <v>61560</v>
       </c>
       <c r="BE7">
-        <f t="shared" si="2"/>
         <v>63099</v>
       </c>
       <c r="BF7">
-        <f t="shared" si="2"/>
         <v>64676.5</v>
       </c>
       <c r="BG7">
-        <f t="shared" si="2"/>
         <v>66293.5</v>
       </c>
       <c r="BH7">
-        <f t="shared" si="2"/>
         <v>67951</v>
       </c>
       <c r="BI7">
-        <f t="shared" si="2"/>
         <v>69649.5</v>
       </c>
       <c r="BJ7">
-        <f t="shared" si="2"/>
         <v>71391</v>
       </c>
       <c r="BK7">
-        <f t="shared" si="2"/>
         <v>73175.5</v>
       </c>
       <c r="BL7">
-        <f t="shared" si="2"/>
         <v>75005</v>
       </c>
       <c r="BM7">
-        <f t="shared" si="2"/>
         <v>76880</v>
       </c>
       <c r="BN7">
-        <f t="shared" si="2"/>
         <v>78802</v>
       </c>
       <c r="BO7">
-        <f t="shared" si="2"/>
         <v>80772.5</v>
       </c>
       <c r="BP7">
-        <f t="shared" si="2"/>
         <v>82791.5</v>
       </c>
       <c r="BQ7">
-        <f t="shared" si="2"/>
         <v>84861.5</v>
       </c>
       <c r="BR7">
-        <f t="shared" ref="BR7:DI7" si="3">BR6*0.5</f>
         <v>86983</v>
       </c>
       <c r="BS7">
-        <f t="shared" si="3"/>
         <v>89157.5</v>
       </c>
       <c r="BT7">
-        <f t="shared" si="3"/>
         <v>91386.5</v>
       </c>
       <c r="BU7">
-        <f t="shared" si="3"/>
         <v>93671</v>
       </c>
       <c r="BV7">
-        <f t="shared" si="3"/>
         <v>96013</v>
       </c>
       <c r="BW7">
-        <f t="shared" si="3"/>
         <v>98413</v>
       </c>
       <c r="BX7">
-        <f t="shared" si="3"/>
         <v>100873.5</v>
       </c>
       <c r="BY7">
-        <f t="shared" si="3"/>
         <v>103395.5</v>
       </c>
       <c r="BZ7">
-        <f t="shared" si="3"/>
         <v>105980</v>
       </c>
       <c r="CA7">
-        <f t="shared" si="3"/>
         <v>108629.5</v>
       </c>
       <c r="CB7">
-        <f t="shared" si="3"/>
         <v>111345.5</v>
       </c>
       <c r="CC7">
-        <f t="shared" si="3"/>
         <v>114129</v>
       </c>
       <c r="CD7">
-        <f t="shared" si="3"/>
         <v>116982.5</v>
       </c>
       <c r="CE7">
-        <f t="shared" si="3"/>
         <v>119907</v>
       </c>
       <c r="CF7">
-        <f t="shared" si="3"/>
         <v>122904.5</v>
       </c>
       <c r="CG7">
-        <f t="shared" si="3"/>
         <v>125977</v>
       </c>
       <c r="CH7">
-        <f t="shared" si="3"/>
         <v>129126.5</v>
       </c>
       <c r="CI7">
-        <f t="shared" si="3"/>
         <v>132354.5</v>
       </c>
       <c r="CJ7">
-        <f t="shared" si="3"/>
         <v>135663.5</v>
       </c>
       <c r="CK7">
-        <f t="shared" si="3"/>
         <v>139055</v>
       </c>
       <c r="CL7">
-        <f t="shared" si="3"/>
         <v>142531.5</v>
       </c>
       <c r="CM7">
-        <f t="shared" si="3"/>
         <v>146095</v>
       </c>
       <c r="CN7">
-        <f t="shared" si="3"/>
         <v>149747</v>
       </c>
       <c r="CO7">
-        <f t="shared" si="3"/>
         <v>153491</v>
       </c>
       <c r="CP7">
-        <f t="shared" si="3"/>
         <v>157328</v>
       </c>
       <c r="CQ7">
-        <f t="shared" si="3"/>
         <v>161261.5</v>
       </c>
       <c r="CR7">
-        <f t="shared" si="3"/>
         <v>165293</v>
       </c>
       <c r="CS7">
-        <f t="shared" si="3"/>
         <v>169425.5</v>
       </c>
       <c r="CT7">
-        <f t="shared" si="3"/>
         <v>173661</v>
       </c>
       <c r="CU7">
-        <f t="shared" si="3"/>
         <v>178002.5</v>
       </c>
       <c r="CV7">
-        <f t="shared" si="3"/>
         <v>182452.5</v>
       </c>
       <c r="CW7">
-        <f t="shared" si="3"/>
         <v>187014</v>
       </c>
       <c r="CX7">
-        <f t="shared" si="3"/>
         <v>191689</v>
       </c>
       <c r="CY7">
-        <f t="shared" si="3"/>
         <v>196481.5</v>
       </c>
       <c r="CZ7">
-        <f t="shared" si="3"/>
         <v>201393.5</v>
       </c>
       <c r="DA7">
-        <f t="shared" si="3"/>
         <v>206428</v>
       </c>
       <c r="DB7">
-        <f t="shared" si="3"/>
         <v>211589</v>
       </c>
       <c r="DC7">
-        <f t="shared" si="3"/>
         <v>216878.5</v>
       </c>
       <c r="DD7">
-        <f t="shared" si="3"/>
         <v>222300.5</v>
       </c>
       <c r="DE7">
-        <f t="shared" si="3"/>
         <v>227858</v>
       </c>
       <c r="DF7">
-        <f t="shared" si="3"/>
         <v>233554.5</v>
       </c>
       <c r="DG7">
-        <f t="shared" si="3"/>
         <v>239393.5</v>
       </c>
       <c r="DH7">
-        <f t="shared" si="3"/>
         <v>245378.5</v>
       </c>
       <c r="DI7">
-        <f t="shared" si="3"/>
         <v>251512.5</v>
       </c>
     </row>
@@ -3096,313 +2878,313 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>3900</v>
+        <v>1950</v>
       </c>
       <c r="L8">
-        <v>3997</v>
+        <v>1998.5</v>
       </c>
       <c r="M8">
-        <v>4097</v>
+        <v>2048.5</v>
       </c>
       <c r="N8">
-        <v>4200</v>
+        <v>2100</v>
       </c>
       <c r="O8">
-        <v>4305</v>
+        <v>2152.5</v>
       </c>
       <c r="P8">
-        <v>4412</v>
+        <v>2206</v>
       </c>
       <c r="Q8">
-        <v>4522</v>
+        <v>2261</v>
       </c>
       <c r="R8">
-        <v>4636</v>
+        <v>2318</v>
       </c>
       <c r="S8">
-        <v>4751</v>
+        <v>2375.5</v>
       </c>
       <c r="T8">
-        <v>4870</v>
+        <v>2435</v>
       </c>
       <c r="U8">
-        <v>4992</v>
+        <v>2496</v>
       </c>
       <c r="V8">
-        <v>6383</v>
+        <v>3191.5</v>
       </c>
       <c r="W8">
-        <v>6543</v>
+        <v>3271.5</v>
       </c>
       <c r="X8">
-        <v>6706</v>
+        <v>3353</v>
       </c>
       <c r="Y8">
-        <v>6874</v>
+        <v>3437</v>
       </c>
       <c r="Z8">
-        <v>7046</v>
+        <v>3523</v>
       </c>
       <c r="AA8">
-        <v>7222</v>
+        <v>3611</v>
       </c>
       <c r="AB8">
-        <v>7402</v>
+        <v>3701</v>
       </c>
       <c r="AC8">
-        <v>7587</v>
+        <v>3793.5</v>
       </c>
       <c r="AD8">
-        <v>7777</v>
+        <v>3888.5</v>
       </c>
       <c r="AE8">
-        <v>7972</v>
+        <v>3986</v>
       </c>
       <c r="AF8">
-        <v>8171</v>
+        <v>4085.5</v>
       </c>
       <c r="AG8">
-        <v>8375</v>
+        <v>4187.5</v>
       </c>
       <c r="AH8">
-        <v>8585</v>
+        <v>4292.5</v>
       </c>
       <c r="AI8">
-        <v>8799</v>
+        <v>4399.5</v>
       </c>
       <c r="AJ8">
-        <v>10356</v>
+        <v>5178</v>
       </c>
       <c r="AK8">
-        <v>10615</v>
+        <v>5307.5</v>
       </c>
       <c r="AL8">
-        <v>10880</v>
+        <v>5440</v>
       </c>
       <c r="AM8">
-        <v>11152</v>
+        <v>5576</v>
       </c>
       <c r="AN8">
-        <v>11431</v>
+        <v>5715.5</v>
       </c>
       <c r="AO8">
-        <v>11717</v>
+        <v>5858.5</v>
       </c>
       <c r="AP8">
-        <v>12010</v>
+        <v>6005</v>
       </c>
       <c r="AQ8">
-        <v>12310</v>
+        <v>6155</v>
       </c>
       <c r="AR8">
-        <v>12618</v>
+        <v>6309</v>
       </c>
       <c r="AS8">
-        <v>12933</v>
+        <v>6466.5</v>
       </c>
       <c r="AT8">
-        <v>13256</v>
+        <v>6628</v>
       </c>
       <c r="AU8">
-        <v>13588</v>
+        <v>6794</v>
       </c>
       <c r="AV8">
-        <v>13927</v>
+        <v>6963.5</v>
       </c>
       <c r="AW8">
-        <v>14276</v>
+        <v>7138</v>
       </c>
       <c r="AX8">
-        <v>14632</v>
+        <v>7316</v>
       </c>
       <c r="AY8">
-        <v>14998</v>
+        <v>7499</v>
       </c>
       <c r="AZ8">
-        <v>15373</v>
+        <v>7686.5</v>
       </c>
       <c r="BA8">
-        <v>15758</v>
+        <v>7879</v>
       </c>
       <c r="BB8">
-        <v>16152</v>
+        <v>8076</v>
       </c>
       <c r="BC8">
-        <v>16555</v>
+        <v>8277.5</v>
       </c>
       <c r="BD8">
-        <v>16969</v>
+        <v>8484.5</v>
       </c>
       <c r="BE8">
-        <v>17393</v>
+        <v>8696.5</v>
       </c>
       <c r="BF8">
-        <v>17828</v>
+        <v>8914</v>
       </c>
       <c r="BG8">
-        <v>18274</v>
+        <v>9137</v>
       </c>
       <c r="BH8">
-        <v>18731</v>
+        <v>9365.5</v>
       </c>
       <c r="BI8">
-        <v>19199</v>
+        <v>9599.5</v>
       </c>
       <c r="BJ8">
-        <v>19679</v>
+        <v>9839.5</v>
       </c>
       <c r="BK8">
-        <v>20171</v>
+        <v>10085.5</v>
       </c>
       <c r="BL8">
-        <v>20675</v>
+        <v>10337.5</v>
       </c>
       <c r="BM8">
-        <v>21192</v>
+        <v>10596</v>
       </c>
       <c r="BN8">
-        <v>21722</v>
+        <v>10861</v>
       </c>
       <c r="BO8">
-        <v>22265</v>
+        <v>11132.5</v>
       </c>
       <c r="BP8">
-        <v>22822</v>
+        <v>11411</v>
       </c>
       <c r="BQ8">
-        <v>23392</v>
+        <v>11696</v>
       </c>
       <c r="BR8">
-        <v>23977</v>
+        <v>11988.5</v>
       </c>
       <c r="BS8">
-        <v>24576</v>
+        <v>12288</v>
       </c>
       <c r="BT8">
-        <v>25191</v>
+        <v>12595.5</v>
       </c>
       <c r="BU8">
-        <v>25821</v>
+        <v>12910.5</v>
       </c>
       <c r="BV8">
-        <v>26466</v>
+        <v>13233</v>
       </c>
       <c r="BW8">
-        <v>27128</v>
+        <v>13564</v>
       </c>
       <c r="BX8">
-        <v>27806</v>
+        <v>13903</v>
       </c>
       <c r="BY8">
-        <v>28501</v>
+        <v>14250.5</v>
       </c>
       <c r="BZ8">
-        <v>29214</v>
+        <v>14607</v>
       </c>
       <c r="CA8">
-        <v>29944</v>
+        <v>14972</v>
       </c>
       <c r="CB8">
-        <v>30693</v>
+        <v>15346.5</v>
       </c>
       <c r="CC8">
-        <v>31460</v>
+        <v>15730</v>
       </c>
       <c r="CD8">
-        <v>32246</v>
+        <v>16123</v>
       </c>
       <c r="CE8">
-        <v>33053</v>
+        <v>16526.5</v>
       </c>
       <c r="CF8">
-        <v>33879</v>
+        <v>16939.5</v>
       </c>
       <c r="CG8">
-        <v>34726</v>
+        <v>17363</v>
       </c>
       <c r="CH8">
-        <v>35594</v>
+        <v>17797</v>
       </c>
       <c r="CI8">
-        <v>36484</v>
+        <v>18242</v>
       </c>
       <c r="CJ8">
-        <v>37396</v>
+        <v>18698</v>
       </c>
       <c r="CK8">
-        <v>38331</v>
+        <v>19165.5</v>
       </c>
       <c r="CL8">
-        <v>39289</v>
+        <v>19644.5</v>
       </c>
       <c r="CM8">
-        <v>40271</v>
+        <v>20135.5</v>
       </c>
       <c r="CN8">
-        <v>41278</v>
+        <v>20639</v>
       </c>
       <c r="CO8">
-        <v>42310</v>
+        <v>21155</v>
       </c>
       <c r="CP8">
-        <v>43368</v>
+        <v>21684</v>
       </c>
       <c r="CQ8">
-        <v>44452</v>
+        <v>22226</v>
       </c>
       <c r="CR8">
-        <v>45563</v>
+        <v>22781.5</v>
       </c>
       <c r="CS8">
-        <v>46702</v>
+        <v>23351</v>
       </c>
       <c r="CT8">
-        <v>47870</v>
+        <v>23935</v>
       </c>
       <c r="CU8">
-        <v>49067</v>
+        <v>24533.5</v>
       </c>
       <c r="CV8">
-        <v>50293</v>
+        <v>25146.5</v>
       </c>
       <c r="CW8">
-        <v>51551</v>
+        <v>25775.5</v>
       </c>
       <c r="CX8">
-        <v>52840</v>
+        <v>26420</v>
       </c>
       <c r="CY8">
-        <v>54161</v>
+        <v>27080.5</v>
       </c>
       <c r="CZ8">
-        <v>55515</v>
+        <v>27757.5</v>
       </c>
       <c r="DA8">
-        <v>56902</v>
+        <v>28451</v>
       </c>
       <c r="DB8">
-        <v>58325</v>
+        <v>29162.5</v>
       </c>
       <c r="DC8">
-        <v>59783</v>
+        <v>29891.5</v>
       </c>
       <c r="DD8">
-        <v>61278</v>
+        <v>30639</v>
       </c>
       <c r="DE8">
-        <v>62810</v>
+        <v>31405</v>
       </c>
       <c r="DF8">
-        <v>64380</v>
+        <v>32190</v>
       </c>
       <c r="DG8">
-        <v>65989</v>
+        <v>32994.5</v>
       </c>
       <c r="DH8">
-        <v>67639</v>
+        <v>33819.5</v>
       </c>
       <c r="DI8">
-        <v>69330</v>
+        <v>34665</v>
       </c>
     </row>
     <row r="9" spans="1:113" x14ac:dyDescent="0.2">
@@ -3419,439 +3201,330 @@
         <v>12</v>
       </c>
       <c r="E9">
-        <f>E8*0.5</f>
         <v>0</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:BQ9" si="4">F8*0.5</f>
         <v>0</v>
       </c>
       <c r="G9">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H9">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J9">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
         <v>1950</v>
       </c>
       <c r="L9">
-        <f t="shared" si="4"/>
         <v>1998.5</v>
       </c>
       <c r="M9">
-        <f t="shared" si="4"/>
         <v>2048.5</v>
       </c>
       <c r="N9">
-        <f t="shared" si="4"/>
         <v>2100</v>
       </c>
       <c r="O9">
-        <f t="shared" si="4"/>
         <v>2152.5</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
         <v>2206</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="4"/>
         <v>2261</v>
       </c>
       <c r="R9">
-        <f t="shared" si="4"/>
         <v>2318</v>
       </c>
       <c r="S9">
-        <f t="shared" si="4"/>
         <v>2375.5</v>
       </c>
       <c r="T9">
-        <f t="shared" si="4"/>
         <v>2435</v>
       </c>
       <c r="U9">
-        <f t="shared" si="4"/>
         <v>2496</v>
       </c>
       <c r="V9">
-        <f t="shared" si="4"/>
         <v>3191.5</v>
       </c>
       <c r="W9">
-        <f t="shared" si="4"/>
         <v>3271.5</v>
       </c>
       <c r="X9">
-        <f t="shared" si="4"/>
         <v>3353</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="4"/>
         <v>3437</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="4"/>
         <v>3523</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="4"/>
         <v>3611</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="4"/>
         <v>3701</v>
       </c>
       <c r="AC9">
-        <f t="shared" si="4"/>
         <v>3793.5</v>
       </c>
       <c r="AD9">
-        <f t="shared" si="4"/>
         <v>3888.5</v>
       </c>
       <c r="AE9">
-        <f t="shared" si="4"/>
         <v>3986</v>
       </c>
       <c r="AF9">
-        <f t="shared" si="4"/>
         <v>4085.5</v>
       </c>
       <c r="AG9">
-        <f t="shared" si="4"/>
         <v>4187.5</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="4"/>
         <v>4292.5</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="4"/>
         <v>4399.5</v>
       </c>
       <c r="AJ9">
-        <f t="shared" si="4"/>
         <v>5178</v>
       </c>
       <c r="AK9">
-        <f t="shared" si="4"/>
         <v>5307.5</v>
       </c>
       <c r="AL9">
-        <f t="shared" si="4"/>
         <v>5440</v>
       </c>
       <c r="AM9">
-        <f t="shared" si="4"/>
         <v>5576</v>
       </c>
       <c r="AN9">
-        <f t="shared" si="4"/>
         <v>5715.5</v>
       </c>
       <c r="AO9">
-        <f t="shared" si="4"/>
         <v>5858.5</v>
       </c>
       <c r="AP9">
-        <f t="shared" si="4"/>
         <v>6005</v>
       </c>
       <c r="AQ9">
-        <f t="shared" si="4"/>
         <v>6155</v>
       </c>
       <c r="AR9">
-        <f t="shared" si="4"/>
         <v>6309</v>
       </c>
       <c r="AS9">
-        <f t="shared" si="4"/>
         <v>6466.5</v>
       </c>
       <c r="AT9">
-        <f t="shared" si="4"/>
         <v>6628</v>
       </c>
       <c r="AU9">
-        <f t="shared" si="4"/>
         <v>6794</v>
       </c>
       <c r="AV9">
-        <f t="shared" si="4"/>
         <v>6963.5</v>
       </c>
       <c r="AW9">
-        <f t="shared" si="4"/>
         <v>7138</v>
       </c>
       <c r="AX9">
-        <f t="shared" si="4"/>
         <v>7316</v>
       </c>
       <c r="AY9">
-        <f t="shared" si="4"/>
         <v>7499</v>
       </c>
       <c r="AZ9">
-        <f t="shared" si="4"/>
         <v>7686.5</v>
       </c>
       <c r="BA9">
-        <f t="shared" si="4"/>
         <v>7879</v>
       </c>
       <c r="BB9">
-        <f t="shared" si="4"/>
         <v>8076</v>
       </c>
       <c r="BC9">
-        <f t="shared" si="4"/>
         <v>8277.5</v>
       </c>
       <c r="BD9">
-        <f t="shared" si="4"/>
         <v>8484.5</v>
       </c>
       <c r="BE9">
-        <f t="shared" si="4"/>
         <v>8696.5</v>
       </c>
       <c r="BF9">
-        <f t="shared" si="4"/>
         <v>8914</v>
       </c>
       <c r="BG9">
-        <f t="shared" si="4"/>
         <v>9137</v>
       </c>
       <c r="BH9">
-        <f t="shared" si="4"/>
         <v>9365.5</v>
       </c>
       <c r="BI9">
-        <f t="shared" si="4"/>
         <v>9599.5</v>
       </c>
       <c r="BJ9">
-        <f t="shared" si="4"/>
         <v>9839.5</v>
       </c>
       <c r="BK9">
-        <f t="shared" si="4"/>
         <v>10085.5</v>
       </c>
       <c r="BL9">
-        <f t="shared" si="4"/>
         <v>10337.5</v>
       </c>
       <c r="BM9">
-        <f t="shared" si="4"/>
         <v>10596</v>
       </c>
       <c r="BN9">
-        <f t="shared" si="4"/>
         <v>10861</v>
       </c>
       <c r="BO9">
-        <f t="shared" si="4"/>
         <v>11132.5</v>
       </c>
       <c r="BP9">
-        <f t="shared" si="4"/>
         <v>11411</v>
       </c>
       <c r="BQ9">
-        <f t="shared" si="4"/>
         <v>11696</v>
       </c>
       <c r="BR9">
-        <f t="shared" ref="BR9:DI9" si="5">BR8*0.5</f>
         <v>11988.5</v>
       </c>
       <c r="BS9">
-        <f t="shared" si="5"/>
         <v>12288</v>
       </c>
       <c r="BT9">
-        <f t="shared" si="5"/>
         <v>12595.5</v>
       </c>
       <c r="BU9">
-        <f t="shared" si="5"/>
         <v>12910.5</v>
       </c>
       <c r="BV9">
-        <f t="shared" si="5"/>
         <v>13233</v>
       </c>
       <c r="BW9">
-        <f t="shared" si="5"/>
         <v>13564</v>
       </c>
       <c r="BX9">
-        <f t="shared" si="5"/>
         <v>13903</v>
       </c>
       <c r="BY9">
-        <f t="shared" si="5"/>
         <v>14250.5</v>
       </c>
       <c r="BZ9">
-        <f t="shared" si="5"/>
         <v>14607</v>
       </c>
       <c r="CA9">
-        <f t="shared" si="5"/>
         <v>14972</v>
       </c>
       <c r="CB9">
-        <f t="shared" si="5"/>
         <v>15346.5</v>
       </c>
       <c r="CC9">
-        <f t="shared" si="5"/>
         <v>15730</v>
       </c>
       <c r="CD9">
-        <f t="shared" si="5"/>
         <v>16123</v>
       </c>
       <c r="CE9">
-        <f t="shared" si="5"/>
         <v>16526.5</v>
       </c>
       <c r="CF9">
-        <f t="shared" si="5"/>
         <v>16939.5</v>
       </c>
       <c r="CG9">
-        <f t="shared" si="5"/>
         <v>17363</v>
       </c>
       <c r="CH9">
-        <f t="shared" si="5"/>
         <v>17797</v>
       </c>
       <c r="CI9">
-        <f t="shared" si="5"/>
         <v>18242</v>
       </c>
       <c r="CJ9">
-        <f t="shared" si="5"/>
         <v>18698</v>
       </c>
       <c r="CK9">
-        <f t="shared" si="5"/>
         <v>19165.5</v>
       </c>
       <c r="CL9">
-        <f t="shared" si="5"/>
         <v>19644.5</v>
       </c>
       <c r="CM9">
-        <f t="shared" si="5"/>
         <v>20135.5</v>
       </c>
       <c r="CN9">
-        <f t="shared" si="5"/>
         <v>20639</v>
       </c>
       <c r="CO9">
-        <f t="shared" si="5"/>
         <v>21155</v>
       </c>
       <c r="CP9">
-        <f t="shared" si="5"/>
         <v>21684</v>
       </c>
       <c r="CQ9">
-        <f t="shared" si="5"/>
         <v>22226</v>
       </c>
       <c r="CR9">
-        <f t="shared" si="5"/>
         <v>22781.5</v>
       </c>
       <c r="CS9">
-        <f t="shared" si="5"/>
         <v>23351</v>
       </c>
       <c r="CT9">
-        <f t="shared" si="5"/>
         <v>23935</v>
       </c>
       <c r="CU9">
-        <f t="shared" si="5"/>
         <v>24533.5</v>
       </c>
       <c r="CV9">
-        <f t="shared" si="5"/>
         <v>25146.5</v>
       </c>
       <c r="CW9">
-        <f t="shared" si="5"/>
         <v>25775.5</v>
       </c>
       <c r="CX9">
-        <f t="shared" si="5"/>
         <v>26420</v>
       </c>
       <c r="CY9">
-        <f t="shared" si="5"/>
         <v>27080.5</v>
       </c>
       <c r="CZ9">
-        <f t="shared" si="5"/>
         <v>27757.5</v>
       </c>
       <c r="DA9">
-        <f t="shared" si="5"/>
         <v>28451</v>
       </c>
       <c r="DB9">
-        <f t="shared" si="5"/>
         <v>29162.5</v>
       </c>
       <c r="DC9">
-        <f t="shared" si="5"/>
         <v>29891.5</v>
       </c>
       <c r="DD9">
-        <f t="shared" si="5"/>
         <v>30639</v>
       </c>
       <c r="DE9">
-        <f t="shared" si="5"/>
         <v>31405</v>
       </c>
       <c r="DF9">
-        <f t="shared" si="5"/>
         <v>32190</v>
       </c>
       <c r="DG9">
-        <f t="shared" si="5"/>
         <v>32994.5</v>
       </c>
       <c r="DH9">
-        <f t="shared" si="5"/>
         <v>33819.5</v>
       </c>
       <c r="DI9">
-        <f t="shared" si="5"/>
         <v>34665</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quite el plural de ....estructura
</commit_message>
<xml_diff>
--- a/app/Datos/Intermodal/Costos e Inversiones.xlsx
+++ b/app/Datos/Intermodal/Costos e Inversiones.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Costos" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="30">
   <si>
     <t>Infraestructura</t>
   </si>
@@ -65,12 +65,6 @@
   </si>
   <si>
     <t>Global</t>
-  </si>
-  <si>
-    <t>Superestructuras</t>
-  </si>
-  <si>
-    <t>Infraestructuras</t>
   </si>
   <si>
     <t>Fase</t>
@@ -449,7 +443,7 @@
   <dimension ref="A1:DI16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:DI16"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,16 +455,16 @@
   <sheetData>
     <row r="1" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1">
         <v>2012</v>
@@ -802,13 +796,13 @@
     </row>
     <row r="2" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -1143,13 +1137,13 @@
     </row>
     <row r="3" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -1484,13 +1478,13 @@
     </row>
     <row r="4" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -1825,13 +1819,13 @@
     </row>
     <row r="5" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -2166,16 +2160,16 @@
     </row>
     <row r="6" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -2507,16 +2501,16 @@
     </row>
     <row r="7" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -2848,16 +2842,16 @@
     </row>
     <row r="8" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3189,16 +3183,16 @@
     </row>
     <row r="9" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -3530,7 +3524,7 @@
     </row>
     <row r="10" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
@@ -3539,7 +3533,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3871,7 +3865,7 @@
     </row>
     <row r="11" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
@@ -3880,7 +3874,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -4212,13 +4206,13 @@
     </row>
     <row r="12" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -4553,13 +4547,13 @@
     </row>
     <row r="13" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
@@ -4894,10 +4888,10 @@
     </row>
     <row r="14" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -5235,13 +5229,13 @@
     </row>
     <row r="15" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
         <v>10</v>
@@ -5576,13 +5570,13 @@
     </row>
     <row r="16" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
         <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
@@ -5936,19 +5930,19 @@
   <sheetData>
     <row r="1" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
-        <v>30</v>
-      </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1">
         <v>2012</v>
@@ -6280,10 +6274,10 @@
     </row>
     <row r="2" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -6292,7 +6286,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -6624,10 +6618,10 @@
     </row>
     <row r="3" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -6636,7 +6630,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -6968,10 +6962,10 @@
     </row>
     <row r="4" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -6980,7 +6974,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -7312,19 +7306,19 @@
     </row>
     <row r="5" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -7656,19 +7650,19 @@
     </row>
     <row r="6" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -8000,19 +7994,19 @@
     </row>
     <row r="7" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -8344,10 +8338,10 @@
     </row>
     <row r="8" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -8356,7 +8350,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -8688,10 +8682,10 @@
     </row>
     <row r="9" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -8700,7 +8694,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -9032,10 +9026,10 @@
     </row>
     <row r="10" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -9044,7 +9038,7 @@
         <v>10</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -9376,19 +9370,19 @@
     </row>
     <row r="11" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -9720,19 +9714,19 @@
     </row>
     <row r="12" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -10064,19 +10058,19 @@
     </row>
     <row r="13" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -10408,7 +10402,7 @@
     </row>
     <row r="14" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -10420,7 +10414,7 @@
         <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -10752,19 +10746,19 @@
     </row>
     <row r="15" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -11096,19 +11090,19 @@
     </row>
     <row r="16" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -11440,19 +11434,19 @@
     </row>
     <row r="17" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
       <c r="E17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -11784,19 +11778,19 @@
     </row>
     <row r="18" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -12128,10 +12122,10 @@
     </row>
     <row r="19" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
@@ -12140,7 +12134,7 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -12472,19 +12466,19 @@
     </row>
     <row r="20" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -12816,10 +12810,10 @@
     </row>
     <row r="21" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
@@ -12828,7 +12822,7 @@
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -13160,19 +13154,19 @@
     </row>
     <row r="22" spans="1:114" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F22">
         <v>0</v>

</xml_diff>